<commit_message>
final commit 2020 assessment
</commit_message>
<xml_diff>
--- a/NSHM/Assessment 2020/results/length/NSHM_size_Based_Indicators_&_Reference_Points_allYears.xlsx
+++ b/NSHM/Assessment 2020/results/length/NSHM_size_Based_Indicators_&_Reference_Points_allYears.xlsx
@@ -1,26 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wageningenur4-my.sharepoint.com/personal/esther_beukhof_wur_nl/Documents/WOT/WGWIDE/NSHM/wg_WGWIDE/NSHM/Assessment 2020/results/length/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beukh001\OneDrive - WageningenUR\WOT\WGWIDE\NSHM\wg_WGWIDE\NSHM\Assessment 2020\results\length\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0FFA10AB-2E8A-45D0-A45A-4EC6A3D35EE7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{345FCFBD-C4A2-45B9-9F2E-ED48FE21B6EF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8352"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8352" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NSHM_size_Based_Indicators_&amp;_Re" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>year</t>
   </si>
@@ -51,11 +54,17 @@
   <si>
     <t>ratio_F_Fmsy</t>
   </si>
+  <si>
+    <t>Countries</t>
+  </si>
+  <si>
+    <t>PFA</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -609,7 +618,17 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.6580927384076991E-2"/>
+          <c:y val="4.6296296296296294E-2"/>
+          <c:w val="0.73482174103237097"/>
+          <c:h val="0.8416746864975212"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -637,7 +656,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -712,7 +743,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -763,6 +806,93 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'NSHM_size_Based_Indicators_&amp;_Re'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'NSHM_size_Based_Indicators_&amp;_Re'!$A$2:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2019</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'NSHM_size_Based_Indicators_&amp;_Re'!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>19.654806001683301</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.134055484083198</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.854405868457199</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.9734699169348</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0650-41D4-BDA0-3E5782F2D984}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -771,6 +901,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="298396296"/>
         <c:axId val="298392032"/>
@@ -830,6 +961,7 @@
         <c:axId val="298392032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="15"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -891,7 +1023,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="t"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -965,7 +1097,626 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Ratio F/FMSY</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'NSHM_size_Based_Indicators_&amp;_Re'!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Countries</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'NSHM_size_Based_Indicators_&amp;_Re'!$A$2:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2019</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'NSHM_size_Based_Indicators_&amp;_Re'!$N$2:$N$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.0843952113684101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0732653074662399</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0482229855762599</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.02547249057845</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-443C-4DA7-8154-2FB3B1E12C53}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'NSHM_size_Based_Indicators_&amp;_Re'!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PFA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'NSHM_size_Based_Indicators_&amp;_Re'!$A$2:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2019</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'NSHM_size_Based_Indicators_&amp;_Re'!$O$2:$O$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.14239641126897</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0504996601462</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0547364938252199</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0450515802161</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-443C-4DA7-8154-2FB3B1E12C53}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="497411616"/>
+        <c:axId val="497413912"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="497411616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Year</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.45677668416447936"/>
+              <c:y val="0.87868037328667248"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="497413912"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="497413912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>F/FMSY</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="497411616"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1521,20 +2272,523 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>163830</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>163830</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1559,7 +2813,82 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>396240</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87638AC8-A898-4FE4-8256-5707560BBE42}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="NSHM_PFA_size_Based_Indicators_"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="J1" t="str">
+            <v>ratio_F_Fmsy</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="J2">
+            <v>1.14239641126897</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="J3">
+            <v>1.0504996601462</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="J4">
+            <v>1.0547364938252199</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="J5">
+            <v>1.0450515802161</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1858,16 +3187,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1898,8 +3227,14 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="N1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2016</v>
       </c>
@@ -1930,8 +3265,17 @@
       <c r="J2">
         <v>1.0843952113684101</v>
       </c>
+      <c r="K2">
+        <v>1.14239641126897</v>
+      </c>
+      <c r="N2">
+        <v>1.0843952113684101</v>
+      </c>
+      <c r="O2">
+        <v>1.14239641126897</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2017</v>
       </c>
@@ -1962,8 +3306,17 @@
       <c r="J3">
         <v>1.0732653074662399</v>
       </c>
+      <c r="K3">
+        <v>1.0504996601462</v>
+      </c>
+      <c r="N3">
+        <v>1.0732653074662399</v>
+      </c>
+      <c r="O3">
+        <v>1.0504996601462</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2018</v>
       </c>
@@ -1994,8 +3347,17 @@
       <c r="J4">
         <v>1.0482229855762599</v>
       </c>
+      <c r="K4">
+        <v>1.0547364938252199</v>
+      </c>
+      <c r="N4">
+        <v>1.0482229855762599</v>
+      </c>
+      <c r="O4">
+        <v>1.0547364938252199</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2019</v>
       </c>
@@ -2025,6 +3387,15 @@
       </c>
       <c r="J5">
         <v>1.02547249057845</v>
+      </c>
+      <c r="K5">
+        <v>1.0450515802161</v>
+      </c>
+      <c r="N5">
+        <v>1.02547249057845</v>
+      </c>
+      <c r="O5">
+        <v>1.0450515802161</v>
       </c>
     </row>
   </sheetData>
@@ -2034,6 +3405,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100959693DDEBB9234399FE2DF0744C4585" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="0378c5d631e9a900a2e387157c0c4b66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d2b4e786-30d2-4c2c-8967-087d16987aff" xmlns:ns4="8ea29b0d-3347-4137-a513-a85c127b091c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5c01a7a8940d80755e6915f64b367bc8" ns3:_="" ns4:_="">
     <xsd:import namespace="d2b4e786-30d2-4c2c-8967-087d16987aff"/>
@@ -2256,22 +3642,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D96DAF9-457A-4193-A4F1-177B5DD327EB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8ea29b0d-3347-4137-a513-a85c127b091c"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d2b4e786-30d2-4c2c-8967-087d16987aff"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00BF6C6E-58EC-41A0-A7B0-BBB3671B26CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DE35629-F800-43E8-A800-467E070EBE05}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2288,29 +3684,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00BF6C6E-58EC-41A0-A7B0-BBB3671B26CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D96DAF9-457A-4193-A4F1-177B5DD327EB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="d2b4e786-30d2-4c2c-8967-087d16987aff"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8ea29b0d-3347-4137-a513-a85c127b091c"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>